<commit_message>
Update Snacks_Fund.xlsx with new data
</commit_message>
<xml_diff>
--- a/Snacks_Fund.xlsx
+++ b/Snacks_Fund.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navneet Chaudhary\Desktop\Fund\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A7189D-D03A-4752-8914-5E03162231F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B8C9CC-9CC5-49BE-B98A-52238A2955FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2560A9AC-C4D8-4295-98D2-145EE83BDA15}"/>
   </bookViews>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>HEMANG JAYESH S</t>
-  </si>
-  <si>
-    <t>HIMANSHU  BHARG</t>
-  </si>
-  <si>
-    <t>SaureenDesai</t>
-  </si>
-  <si>
-    <t>PRAJAPATI DIPTI</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Preety</t>
   </si>
@@ -68,9 +56,6 @@
     <t>Snacks</t>
   </si>
   <si>
-    <t>Ranjeet sharma</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -78,12 +63,30 @@
   </si>
   <si>
     <t>Contribution</t>
+  </si>
+  <si>
+    <t>Hemang Jayesh S</t>
+  </si>
+  <si>
+    <t>Himanshu  Bharg</t>
+  </si>
+  <si>
+    <t>Saureendesai</t>
+  </si>
+  <si>
+    <t>Prajapati Dipti</t>
+  </si>
+  <si>
+    <t>Ranjeet Sharma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="&quot;₹&quot;\ #,##0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -160,10 +163,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +507,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,31 +515,32 @@
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
@@ -544,13 +551,13 @@
         <v>45766</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12">
         <v>500</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="12">
         <f>E2-D2</f>
         <v>500</v>
       </c>
@@ -564,34 +571,34 @@
         <v>45766</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7">
+        <v>10</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12">
         <v>500</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="12">
         <f>F2+E3-D3</f>
         <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A12" si="0">A3+1</f>
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="6">
         <v>45766</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12">
         <v>500</v>
       </c>
-      <c r="F4" s="8">
-        <f t="shared" ref="F4:F12" si="1">F3+E4-D4</f>
+      <c r="F4" s="12">
+        <f t="shared" ref="F4:F9" si="1">F3+E4-D4</f>
         <v>1500</v>
       </c>
     </row>
@@ -604,13 +611,13 @@
         <v>45766</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7">
+        <v>12</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12">
         <v>500</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="12">
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
@@ -624,13 +631,13 @@
         <v>45766</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12">
         <v>500</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="12">
         <f t="shared" si="1"/>
         <v>2500</v>
       </c>
@@ -644,13 +651,13 @@
         <v>45766</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12">
         <v>500</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="12">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
@@ -664,17 +671,16 @@
         <v>45766</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7">
+        <v>13</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12">
         <v>536</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="12">
         <f t="shared" si="1"/>
         <v>3536</v>
       </c>
-      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -685,78 +691,31 @@
         <v>45766</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12">
         <v>536</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45767</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="11">
-        <v>1000</v>
-      </c>
-      <c r="F10" s="8">
-        <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <f>B10+1</f>
-        <v>45768</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="11">
-        <v>5000</v>
-      </c>
-      <c r="F11" s="8">
-        <f t="shared" si="1"/>
-        <v>9000</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <f>B11+1</f>
-        <v>45769</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7">
-        <v>2000</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8">
-        <f t="shared" si="1"/>
-        <v>7000</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="F12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>